<commit_message>
Git excel zarez and track the rest 2 files
</commit_message>
<xml_diff>
--- a/Git.xlsx
+++ b/Git.xlsx
@@ -945,10 +945,10 @@
     <t>git log --oneline --graph</t>
   </si>
   <si>
-    <t>git log --pretty="%h, %cn %cr"</t>
-  </si>
-  <si>
     <t>(abbriviated) hash, committer name,  time elapsed since commit taken</t>
+  </si>
+  <si>
+    <t>git log --pretty="%h, %cn, %cr"</t>
   </si>
 </sst>
 </file>
@@ -4223,7 +4223,7 @@
   <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4256,10 +4256,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" s="23" t="s">
         <v>133</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>134</v>
       </c>
       <c r="C3" s="22"/>
     </row>

</xml_diff>